<commit_message>
move folders and edit input_gui.py
</commit_message>
<xml_diff>
--- a/prj_input/src_input_gui/test_data.xlsx
+++ b/prj_input/src_input_gui/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Toshiaki/Desktop/rakutto_collect_project/prj_input/src_input_gui/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4193D98C-E0A6-A04F-816B-B2E3A70C93FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603D5FB0-29A7-4840-A779-F1A2437847AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4040" yWindow="-20780" windowWidth="21600" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26240" yWindow="-13380" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="患者情報入力シート" sheetId="8" r:id="rId1"/>
@@ -1331,11 +1331,11 @@
   </sheetPr>
   <dimension ref="A1:AJ272"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="15" ySplit="2" topLeftCell="AF3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="15" ySplit="2" topLeftCell="AE3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomRight" activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1"/>
@@ -13913,8 +13913,8 @@
   </sheetPr>
   <dimension ref="A1:AA1054"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1"/>

</xml_diff>

<commit_message>
debugging is started. Values are not correctly installed.  Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/prj_input/src_input_gui/test_data.xlsx
+++ b/prj_input/src_input_gui/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Toshiaki/Desktop/rakutto_collect_project/prj_input/src_input_gui/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603D5FB0-29A7-4840-A779-F1A2437847AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FA3D96-4407-F943-B48E-8A61F6583510}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26240" yWindow="-13380" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28160" yWindow="-6180" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="患者情報入力シート" sheetId="8" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="150">
   <si>
     <t>保健所</t>
   </si>
@@ -128,13 +128,6 @@
   </si>
   <si>
     <t>90-99歳</t>
-  </si>
-  <si>
-    <t>日付</t>
-    <rPh sb="0" eb="2">
-      <t>ヒヅケ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>01_会社員</t>
@@ -670,6 +663,9 @@
   <si>
     <t>https://mmm-program.com/vba-userform-mousescroll/</t>
     <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>日付</t>
   </si>
 </sst>
 </file>
@@ -1331,11 +1327,11 @@
   </sheetPr>
   <dimension ref="A1:AJ272"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="15" ySplit="2" topLeftCell="AE3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="15" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AG18" sqref="AG18"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1"/>
@@ -1470,10 +1466,10 @@
     </row>
     <row r="2" spans="1:36" s="40" customFormat="1" ht="49.5" customHeight="1">
       <c r="A2" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="31" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>57</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>1</v>
@@ -1482,13 +1478,13 @@
         <v>2</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="39" t="s">
         <v>4</v>
@@ -1503,10 +1499,10 @@
         <v>6</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M2" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N2" s="39" t="s">
         <v>0</v>
@@ -1515,10 +1511,10 @@
         <v>8</v>
       </c>
       <c r="P2" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q2" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R2" s="31" t="s">
         <v>1</v>
@@ -1527,13 +1523,13 @@
         <v>2</v>
       </c>
       <c r="T2" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="U2" s="31" t="s">
         <v>3</v>
       </c>
       <c r="V2" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W2" s="39" t="s">
         <v>4</v>
@@ -1548,19 +1544,19 @@
         <v>6</v>
       </c>
       <c r="AA2" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB2" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC2" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="AC2" s="31" t="s">
-        <v>74</v>
-      </c>
       <c r="AD2" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AE2" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AF2" s="39" t="s">
         <v>14</v>
@@ -1569,7 +1565,7 @@
         <v>15</v>
       </c>
       <c r="AH2" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:36" s="42" customFormat="1" ht="18.75" customHeight="1">
@@ -1579,9 +1575,7 @@
       <c r="B3" s="43">
         <v>43924</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>147</v>
-      </c>
+      <c r="C3" s="12"/>
       <c r="D3" s="27"/>
       <c r="E3" s="44"/>
       <c r="F3" s="27"/>
@@ -1591,13 +1585,13 @@
       <c r="J3" s="27"/>
       <c r="K3" s="44"/>
       <c r="L3" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M3" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N3" s="43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O3" s="43"/>
       <c r="P3" s="32">
@@ -1607,36 +1601,36 @@
         <v>78</v>
       </c>
       <c r="R3" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S3" s="27"/>
       <c r="T3" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="U3" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="U3" s="27" t="s">
-        <v>133</v>
-      </c>
       <c r="V3" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W3" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X3" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Y3" s="27"/>
       <c r="Z3" s="44" t="s">
         <v>17</v>
       </c>
       <c r="AA3" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB3" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC3" s="27" t="s">
         <v>87</v>
-      </c>
-      <c r="AC3" s="27" t="s">
-        <v>88</v>
       </c>
       <c r="AD3" s="27" t="s">
         <v>17</v>
@@ -1660,73 +1654,73 @@
         <v>43891</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E4" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>133</v>
-      </c>
       <c r="G4" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H4" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J4" s="27"/>
       <c r="K4" s="44" t="s">
         <v>17</v>
       </c>
       <c r="L4" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M4" s="27"/>
       <c r="N4" s="43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O4" s="43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P4" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q4" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="Q4" s="33" t="s">
-        <v>137</v>
-      </c>
       <c r="R4" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="S4" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="T4" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="S4" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="T4" s="44" t="s">
+      <c r="U4" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="U4" s="27" t="s">
-        <v>133</v>
-      </c>
       <c r="V4" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W4" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X4" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Y4" s="27"/>
       <c r="Z4" s="44" t="s">
         <v>17</v>
       </c>
       <c r="AA4" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AB4" s="27"/>
       <c r="AC4" s="27"/>
@@ -1734,7 +1728,7 @@
         <v>17</v>
       </c>
       <c r="AE4" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AF4" s="43">
         <v>43905</v>
@@ -1746,77 +1740,69 @@
     </row>
     <row r="5" spans="1:36" s="42" customFormat="1" ht="18.75" customHeight="1">
       <c r="A5" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="43" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>131</v>
-      </c>
+      <c r="C5" s="12"/>
       <c r="D5" s="27"/>
-      <c r="E5" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="G5" s="44" t="s">
-        <v>132</v>
-      </c>
+      <c r="E5" s="44"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="44"/>
       <c r="H5" s="43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J5" s="27"/>
       <c r="K5" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L5" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M5" s="27"/>
       <c r="N5" s="43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O5" s="43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P5" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q5" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="Q5" s="33" t="s">
-        <v>141</v>
-      </c>
       <c r="R5" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="S5" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="T5" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="S5" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="T5" s="44" t="s">
+      <c r="U5" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="U5" s="27" t="s">
-        <v>133</v>
-      </c>
       <c r="V5" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="W5" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X5" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Y5" s="27"/>
       <c r="Z5" s="44" t="s">
         <v>17</v>
       </c>
       <c r="AA5" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AB5" s="27"/>
       <c r="AC5" s="27"/>
@@ -1824,7 +1810,7 @@
         <v>17</v>
       </c>
       <c r="AE5" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AF5" s="43">
         <v>43909</v>
@@ -1849,27 +1835,27 @@
         <v>17</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G6" s="44" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J6" s="27"/>
       <c r="K6" s="44" t="s">
         <v>17</v>
       </c>
       <c r="L6" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M6" s="27"/>
       <c r="N6" s="43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O6" s="43"/>
       <c r="P6" s="32">
@@ -1886,23 +1872,23 @@
         <v>17</v>
       </c>
       <c r="U6" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V6" s="44" t="s">
         <v>17</v>
       </c>
       <c r="W6" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X6" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Y6" s="27"/>
       <c r="Z6" s="44" t="s">
         <v>17</v>
       </c>
       <c r="AA6" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AB6" s="27"/>
       <c r="AC6" s="27"/>
@@ -1910,7 +1896,7 @@
         <v>17</v>
       </c>
       <c r="AE6" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AF6" s="43">
         <v>43908</v>
@@ -1935,27 +1921,27 @@
         <v>28</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G7" s="44" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J7" s="27"/>
       <c r="K7" s="44" t="s">
         <v>28</v>
       </c>
       <c r="L7" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M7" s="27"/>
       <c r="N7" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O7" s="43"/>
       <c r="P7" s="32">
@@ -1972,23 +1958,23 @@
         <v>28</v>
       </c>
       <c r="U7" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V7" s="44" t="s">
         <v>17</v>
       </c>
       <c r="W7" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X7" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Y7" s="27"/>
       <c r="Z7" s="44" t="s">
         <v>28</v>
       </c>
       <c r="AA7" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AB7" s="27"/>
       <c r="AC7" s="27"/>
@@ -2014,34 +2000,34 @@
         <v>43903</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="44" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G8" s="44" t="s">
         <v>17</v>
       </c>
       <c r="H8" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J8" s="27"/>
       <c r="K8" s="44" t="s">
         <v>17</v>
       </c>
       <c r="L8" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M8" s="27"/>
       <c r="N8" s="43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O8" s="43"/>
       <c r="P8" s="32">
@@ -2058,23 +2044,23 @@
         <v>17</v>
       </c>
       <c r="U8" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V8" s="44" t="s">
         <v>17</v>
       </c>
       <c r="W8" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X8" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Y8" s="27"/>
       <c r="Z8" s="44" t="s">
         <v>17</v>
       </c>
       <c r="AA8" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AB8" s="27"/>
       <c r="AC8" s="27"/>
@@ -2094,40 +2080,40 @@
     </row>
     <row r="9" spans="1:36" s="42" customFormat="1" ht="18.75" customHeight="1">
       <c r="A9" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="C9" s="12" t="s">
         <v>146</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>147</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="44" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G9" s="44" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J9" s="27"/>
       <c r="K9" s="44" t="s">
         <v>17</v>
       </c>
       <c r="L9" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M9" s="27"/>
       <c r="N9" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O9" s="43"/>
       <c r="P9" s="32">
@@ -2144,23 +2130,23 @@
         <v>17</v>
       </c>
       <c r="U9" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V9" s="44" t="s">
         <v>17</v>
       </c>
       <c r="W9" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X9" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Y9" s="27"/>
       <c r="Z9" s="44" t="s">
         <v>17</v>
       </c>
       <c r="AA9" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AB9" s="27"/>
       <c r="AC9" s="27"/>
@@ -2168,7 +2154,7 @@
         <v>17</v>
       </c>
       <c r="AE9" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AF9" s="43">
         <v>43920</v>
@@ -2193,27 +2179,27 @@
         <v>17</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G10" s="44" t="s">
         <v>17</v>
       </c>
       <c r="H10" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J10" s="27"/>
       <c r="K10" s="44" t="s">
         <v>17</v>
       </c>
       <c r="L10" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M10" s="27"/>
       <c r="N10" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O10" s="43"/>
       <c r="P10" s="32">
@@ -2230,23 +2216,23 @@
         <v>17</v>
       </c>
       <c r="U10" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V10" s="44" t="s">
         <v>17</v>
       </c>
       <c r="W10" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X10" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Y10" s="27"/>
       <c r="Z10" s="44" t="s">
         <v>17</v>
       </c>
       <c r="AA10" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AB10" s="27"/>
       <c r="AC10" s="27"/>
@@ -2254,7 +2240,7 @@
         <v>17</v>
       </c>
       <c r="AE10" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AF10" s="43"/>
       <c r="AG10" s="27"/>
@@ -2277,29 +2263,29 @@
         <v>17</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G11" s="44" t="s">
         <v>17</v>
       </c>
       <c r="H11" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J11" s="27"/>
       <c r="K11" s="44" t="s">
         <v>17</v>
       </c>
       <c r="L11" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M11" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N11" s="43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O11" s="43"/>
       <c r="P11" s="32">
@@ -2316,33 +2302,33 @@
         <v>17</v>
       </c>
       <c r="U11" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="V11" s="44" t="s">
         <v>17</v>
       </c>
       <c r="W11" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X11" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Y11" s="27"/>
       <c r="Z11" s="44" t="s">
         <v>17</v>
       </c>
       <c r="AA11" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB11" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AC11" s="27"/>
       <c r="AD11" s="27" t="s">
         <v>17</v>
       </c>
       <c r="AE11" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AF11" s="43"/>
       <c r="AG11" s="27"/>
@@ -2365,27 +2351,27 @@
         <v>17</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G12" s="44" t="s">
         <v>17</v>
       </c>
       <c r="H12" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J12" s="27"/>
       <c r="K12" s="44" t="s">
         <v>17</v>
       </c>
       <c r="L12" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M12" s="27"/>
       <c r="N12" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O12" s="43"/>
       <c r="P12" s="32">
@@ -2402,23 +2388,23 @@
         <v>17</v>
       </c>
       <c r="U12" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="V12" s="44" t="s">
         <v>17</v>
       </c>
       <c r="W12" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="X12" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Y12" s="27"/>
       <c r="Z12" s="44" t="s">
         <v>17</v>
       </c>
       <c r="AA12" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AB12" s="27"/>
       <c r="AC12" s="27"/>
@@ -2426,7 +2412,7 @@
         <v>17</v>
       </c>
       <c r="AE12" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AF12" s="43"/>
       <c r="AG12" s="27"/>
@@ -13913,8 +13899,8 @@
   </sheetPr>
   <dimension ref="A1:AA1054"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1"/>
@@ -13938,10 +13924,10 @@
   <sheetData>
     <row r="1" spans="1:27" s="34" customFormat="1" ht="18.75" customHeight="1">
       <c r="A1" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>32</v>
+        <v>149</v>
       </c>
       <c r="C1" s="30">
         <v>5</v>
@@ -13953,34 +13939,34 @@
         <v>7</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G1" s="30">
         <v>9</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J1" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K1" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L1" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M1" s="30">
         <v>15</v>
       </c>
       <c r="N1" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O1" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P1" s="30">
         <v>18</v>
@@ -13989,25 +13975,25 @@
         <v>19</v>
       </c>
       <c r="R1" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S1" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T1" s="30">
         <v>22</v>
       </c>
       <c r="U1" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="V1" s="30">
         <v>24</v>
       </c>
       <c r="W1" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X1" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Y1" s="30">
         <v>63</v>
@@ -14021,19 +14007,19 @@
     </row>
     <row r="2" spans="1:27" s="38" customFormat="1" ht="53.25" customHeight="1">
       <c r="A2" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="35" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>57</v>
       </c>
       <c r="C2" s="36" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" s="35" t="s">
         <v>1</v>
@@ -14042,13 +14028,13 @@
         <v>2</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I2" s="35" t="s">
         <v>3</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K2" s="36" t="s">
         <v>4</v>
@@ -14063,19 +14049,19 @@
         <v>6</v>
       </c>
       <c r="O2" s="37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P2" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="Q2" s="37" t="s">
-        <v>74</v>
-      </c>
       <c r="R2" s="35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S2" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T2" s="35" t="s">
         <v>9</v>
@@ -14099,7 +14085,7 @@
         <v>15</v>
       </c>
       <c r="AA2" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="18.75" customHeight="1">
@@ -14109,28 +14095,28 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -14138,7 +14124,7 @@
         <v>17</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2" t="s">
@@ -14149,7 +14135,7 @@
         <v>21</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="18.75" customHeight="1">
@@ -14165,22 +14151,22 @@
         <v>28</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -14188,7 +14174,7 @@
         <v>28</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T4" s="2"/>
       <c r="U4" s="2" t="s">
@@ -14199,7 +14185,7 @@
         <v>19</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="18.75" customHeight="1">
@@ -14212,22 +14198,22 @@
         <v>30</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T5" s="2"/>
       <c r="V5" s="2"/>
@@ -14246,22 +14232,22 @@
         <v>29</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T6" s="2"/>
       <c r="V6" s="2"/>
@@ -14278,14 +14264,14 @@
         <v>16</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T7" s="2"/>
       <c r="V7" s="2"/>
@@ -14302,7 +14288,7 @@
         <v>20</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M8" s="4"/>
       <c r="O8" s="2"/>
@@ -14310,7 +14296,7 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T8" s="2"/>
       <c r="V8" s="2"/>
@@ -14327,7 +14313,7 @@
         <v>23</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M9" s="4"/>
       <c r="O9" s="2"/>
@@ -14335,7 +14321,7 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T9" s="2"/>
       <c r="V9" s="2"/>
@@ -14352,7 +14338,7 @@
         <v>25</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M10" s="4"/>
       <c r="O10" s="2"/>
@@ -14360,7 +14346,7 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T10" s="2"/>
       <c r="V10" s="2"/>
@@ -14377,7 +14363,7 @@
         <v>27</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M11" s="4"/>
       <c r="O11" s="2"/>
@@ -14385,7 +14371,7 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T11" s="2"/>
       <c r="V11" s="2"/>
@@ -14422,7 +14408,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
@@ -20052,198 +20038,198 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I2" s="48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17">
       <c r="A4" s="41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16">
       <c r="A7" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="21">
       <c r="A13" s="47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="48" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="17">
       <c r="A25" s="41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new line function is added.
Next thing is that layout is changed,
so that users can easily use it.
</commit_message>
<xml_diff>
--- a/prj_input/src_input_gui/test_data.xlsx
+++ b/prj_input/src_input_gui/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Toshiaki/Desktop/rakutto_collect_project/prj_input/src_input_gui/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291E3EBD-D9C8-FE49-9B14-1AD8AE66D977}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CB6171-CF69-2648-A1D7-2FC35232091F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28160" yWindow="-6180" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4700" yWindow="-16580" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="患者情報入力シート" sheetId="8" r:id="rId1"/>
@@ -1283,7 +1283,7 @@
       <pane xSplit="15" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V9" sqref="V9"/>
+      <selection pane="bottomRight" activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18.75" customHeight="1"/>

</xml_diff>